<commit_message>
Everything done but images
</commit_message>
<xml_diff>
--- a/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
+++ b/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b062fc832ee273/Work/BusiHealth ^0 BusiVet/Site Report Automator/pdf_report_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{197A8843-8B24-514D-BBFF-F99EF0A02C9B}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEB7F948-3AB4-8E43-935C-699E2BAAC52F}"/>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="-21600" windowWidth="13260" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20340" yWindow="-21100" windowWidth="13260" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,158 @@
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="14">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="14">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,483 +871,152 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 5" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 8" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 9" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 10" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Image 11" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 12" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Image 2" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4363F19-2999-A54D-BCA1-C854E2AC684F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1168977" y="1385455"/>
-          <a:ext cx="1428750" cy="1143000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1428750" cy="1143000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Image 9" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C74832E-7DD8-CD43-9EF7-2C36B9745A4E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1168977" y="9611591"/>
-          <a:ext cx="1428750" cy="1143000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+    <k n="Text" t="s"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1485,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="BD2" sqref="BD2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1726,7 +1547,9 @@
       <c r="A2" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>173</v>
       </c>
@@ -1878,7 +1701,9 @@
       <c r="A3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>77</v>
       </c>
@@ -2026,7 +1851,9 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>85</v>
       </c>
@@ -2176,7 +2003,9 @@
       <c r="A5" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
       <c r="C5" s="5" t="s">
         <v>94</v>
       </c>
@@ -2324,7 +2153,9 @@
       <c r="A6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
       <c r="C6" s="5" t="s">
         <v>102</v>
       </c>
@@ -2472,7 +2303,9 @@
       <c r="A7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
       <c r="C7" s="5" t="s">
         <v>109</v>
       </c>
@@ -2622,7 +2455,9 @@
       <c r="A8" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>117</v>
       </c>
@@ -2772,7 +2607,9 @@
       <c r="A9" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>147</v>
       </c>
@@ -2926,7 +2763,9 @@
       <c r="A10" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
       <c r="C10" s="5" t="s">
         <v>130</v>
       </c>
@@ -3078,7 +2917,9 @@
       <c r="A11" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>165</v>
       </c>
@@ -3232,7 +3073,9 @@
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
       <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
@@ -3380,7 +3223,9 @@
       <c r="A13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
       <c r="C13" s="5" t="s">
         <v>125</v>
       </c>
@@ -3528,7 +3373,9 @@
       <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
       <c r="C14" s="5" t="s">
         <v>130</v>
       </c>
@@ -3678,7 +3525,9 @@
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
       <c r="C15" s="5" t="s">
         <v>136</v>
       </c>
@@ -3848,6 +3697,5 @@
     <hyperlink ref="Y2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Version - images blury but they need to be manually put in
</commit_message>
<xml_diff>
--- a/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
+++ b/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b062fc832ee273/Work/BusiHealth ^0 BusiVet/Site Report Automator/pdf_report_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEB7F948-3AB4-8E43-935C-699E2BAAC52F}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23A4A6A-C582-5341-9F88-7FEB6911A754}"/>
   <bookViews>
     <workbookView xWindow="20340" yWindow="-21100" windowWidth="13260" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="14">
+  <futureMetadata name="XLRICHVALUE" count="13">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -119,15 +119,8 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="13"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="14">
+  <valueMetadata count="13">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -166,9 +159,6 @@
     </bk>
     <bk>
       <rc t="1" v="12"/>
-    </bk>
-    <bk>
-      <rc t="1" v="13"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -871,6 +861,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C845DEBF-AB0B-8E74-86B2-A2188B3EB121}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1168712" y="7355092"/>
+          <a:ext cx="1435100" cy="1155700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -916,7 +955,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -982,11 +1021,6 @@
     <v>5</v>
     <v>Picture</v>
   </rv>
-  <rv s="0">
-    <v>13</v>
-    <v>5</v>
-    <v>Picture</v>
-  </rv>
 </rvData>
 </file>
 
@@ -1015,7 +1049,6 @@
   <rel r:id="rId11"/>
   <rel r:id="rId12"/>
   <rel r:id="rId13"/>
-  <rel r:id="rId14"/>
 </richValueRels>
 </file>
 
@@ -1306,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2607,9 +2640,7 @@
       <c r="A9" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="5" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
         <v>147</v>
       </c>
@@ -2763,7 +2794,7 @@
       <c r="A10" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="5" t="e" vm="9">
+      <c r="B10" s="5" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2917,7 +2948,7 @@
       <c r="A11" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="5" t="e" vm="10">
+      <c r="B11" s="5" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -3073,7 +3104,7 @@
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="5" t="e" vm="11">
+      <c r="B12" s="5" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -3223,7 +3254,7 @@
       <c r="A13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="5" t="e" vm="12">
+      <c r="B13" s="5" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3373,7 +3404,7 @@
       <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="5" t="e" vm="13">
+      <c r="B14" s="5" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3525,7 +3556,7 @@
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5" t="e" vm="14">
+      <c r="B15" s="5" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3697,5 +3728,6 @@
     <hyperlink ref="Y2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Windows setup file run_windows.bat - double click to install and run everything
</commit_message>
<xml_diff>
--- a/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
+++ b/Properties_Hunters_Hill_NSW_2110_Crows_Nest_NSW_2065_04_04_2025_18_03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b062fc832ee273/Work/BusiHealth ^0 BusiVet/Site Report Automator/pdf_report_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C23A4A6A-C582-5341-9F88-7FEB6911A754}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{E5B26731-5F14-414C-85BA-EAD721713F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9D121CE-F572-7647-A948-30F8705656D7}"/>
   <bookViews>
     <workbookView xWindow="20340" yWindow="-21100" windowWidth="13260" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="13">
+  <futureMetadata name="XLRICHVALUE" count="14">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -119,8 +119,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="13">
+  <valueMetadata count="14">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -159,6 +166,9 @@
     </bk>
     <bk>
       <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -861,55 +871,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1435100</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>10363</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C845DEBF-AB0B-8E74-86B2-A2188B3EB121}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1168712" y="7355092"/>
-          <a:ext cx="1435100" cy="1155700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -955,7 +916,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="13">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="14">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1021,6 +982,11 @@
     <v>5</v>
     <v>Picture</v>
   </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+    <v>Picture</v>
+  </rv>
 </rvData>
 </file>
 
@@ -1049,6 +1015,7 @@
   <rel r:id="rId11"/>
   <rel r:id="rId12"/>
   <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
 </richValueRels>
 </file>
 
@@ -1339,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="163" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="93" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2640,7 +2607,9 @@
       <c r="A9" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
       <c r="C9" s="5" t="s">
         <v>147</v>
       </c>
@@ -2794,7 +2763,7 @@
       <c r="A10" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="5" t="e" vm="8">
+      <c r="B10" s="5" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2948,7 +2917,7 @@
       <c r="A11" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="5" t="e" vm="9">
+      <c r="B11" s="5" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -3104,7 +3073,7 @@
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="5" t="e" vm="10">
+      <c r="B12" s="5" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -3254,7 +3223,7 @@
       <c r="A13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="5" t="e" vm="11">
+      <c r="B13" s="5" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -3404,7 +3373,7 @@
       <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="5" t="e" vm="12">
+      <c r="B14" s="5" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -3556,7 +3525,7 @@
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5" t="e" vm="13">
+      <c r="B15" s="5" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -3728,6 +3697,5 @@
     <hyperlink ref="Y2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>